<commit_message>
Externally linked image urls
</commit_message>
<xml_diff>
--- a/documentation/Metadata Form, Item Type, Subjects.xlsx
+++ b/documentation/Metadata Form, Item Type, Subjects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\British Library\bl github group\bl_github_clones\idp-data-issues\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F752A9-A35E-4BD7-A1CB-AD4D6CB230B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D0330A-CBDC-4EDA-96A8-057AC7AF1E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2412" yWindow="7908" windowWidth="19800" windowHeight="18648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2412" yWindow="6552" windowWidth="19800" windowHeight="18648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FORM" sheetId="1" r:id="rId1"/>
@@ -2216,7 +2216,7 @@
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
     </row>
-    <row r="6" spans="1:10" ht="96.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>18</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="124.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="69" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>21</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="124.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="69" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>45</v>
       </c>
@@ -3260,7 +3260,7 @@
       <c r="I47" s="18"/>
       <c r="J47" s="18"/>
     </row>
-    <row r="48" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>77</v>
       </c>
@@ -3808,7 +3808,7 @@
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
     </row>
-    <row r="72" spans="1:10" ht="69" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A72" s="15" t="s">
         <v>104</v>
       </c>

</xml_diff>